<commit_message>
now we can lock the pos shft to calc
</commit_message>
<xml_diff>
--- a/input_sample/M18104948C/M18104948C_input_df.xlsx
+++ b/input_sample/M18104948C/M18104948C_input_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="88">
   <si>
     <t>en_width</t>
   </si>
@@ -70,7 +70,7 @@
     <t>prf_fin</t>
   </si>
   <si>
-    <t>wr_shft</t>
+    <t>wr_shft_lock</t>
   </si>
   <si>
     <t>force_bnd</t>
@@ -269,15 +269,6 @@
   </si>
   <si>
     <t xml:space="preserve">0.0519 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   26.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -85.94</t>
   </si>
   <si>
     <t xml:space="preserve">   890</t>
@@ -773,14 +764,11 @@
       <c r="S2" t="s">
         <v>84</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>85</v>
       </c>
-      <c r="U2" t="s">
-        <v>88</v>
-      </c>
       <c r="V2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -841,14 +829,11 @@
       <c r="S3" t="s">
         <v>84</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>85</v>
       </c>
-      <c r="U3" t="s">
-        <v>88</v>
-      </c>
       <c r="V3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -909,14 +894,11 @@
       <c r="S4" t="s">
         <v>84</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>85</v>
       </c>
-      <c r="U4" t="s">
-        <v>88</v>
-      </c>
       <c r="V4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -977,14 +959,11 @@
       <c r="S5" t="s">
         <v>84</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>85</v>
       </c>
-      <c r="U5" t="s">
-        <v>88</v>
-      </c>
       <c r="V5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -1045,14 +1024,11 @@
       <c r="S6" t="s">
         <v>84</v>
       </c>
-      <c r="T6" t="s">
-        <v>85</v>
-      </c>
       <c r="U6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="V6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1113,14 +1089,11 @@
       <c r="S7" t="s">
         <v>84</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>86</v>
       </c>
-      <c r="U7" t="s">
-        <v>89</v>
-      </c>
       <c r="V7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1181,14 +1154,11 @@
       <c r="S8" t="s">
         <v>84</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
+        <v>86</v>
+      </c>
+      <c r="V8" t="s">
         <v>87</v>
-      </c>
-      <c r="U8" t="s">
-        <v>89</v>
-      </c>
-      <c r="V8" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>